<commit_message>
spreadsheet licenses and is_isPartOf updated
</commit_message>
<xml_diff>
--- a/content/resources/user-guides/crate-o/spreadsheet-upload/ro-crate-metadata-template.xlsx
+++ b/content/resources/user-guides/crate-o/spreadsheet-upload/ro-crate-metadata-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rosannasmith/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4233410D-8307-FF41-A9AD-EE2674A8634E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01926BD-2AF4-F740-AC3D-FF32CD4078D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17480" yWindow="18940" windowWidth="33020" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5940" yWindow="5280" windowWidth="32900" windowHeight="20220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="10" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="56">
   <si>
     <t>@id</t>
   </si>
@@ -61,9 +61,6 @@
     <t>isRef_annotationOf</t>
   </si>
   <si>
-    <t>isRef_partOf</t>
-  </si>
-  <si>
     <t>Female</t>
   </si>
   <si>
@@ -160,9 +157,6 @@
     <t>ExampleCollection_Speaker_01</t>
   </si>
   <si>
-    <t>ExampleCollection_Speaker_01.wav</t>
-  </si>
-  <si>
     <t>Audio</t>
   </si>
   <si>
@@ -209,12 +203,21 @@
   </si>
   <si>
     <t>DataReuseLicense</t>
+  </si>
+  <si>
+    <t>Audio/ExampleCollection_Speaker_01.wav</t>
+  </si>
+  <si>
+    <t>isRef_isPartOf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
   <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -898,7 +901,6 @@
     <xf numFmtId="0" fontId="27" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="27" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="42" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -906,6 +908,7 @@
     <xf numFmtId="0" fontId="16" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="27" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="58">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1283,11 +1286,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B1B4B01-7DA1-4F69-8EF2-3B9D5666F67A}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1298,46 +1301,50 @@
     <col min="5" max="5" width="25.5" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" customWidth="1"/>
     <col min="7" max="7" width="22.6640625" customWidth="1"/>
+    <col min="8" max="8" width="40.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="21" t="s">
+      <c r="D1" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="H1" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="16" t="s">
+      <c r="E2" s="16" t="s">
         <v>32</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>33</v>
       </c>
       <c r="F2" s="15" t="str">
         <f>AUTHORS!A2</f>
@@ -1346,6 +1353,10 @@
       <c r="G2" s="15" t="str">
         <f>PUBLISHERS!A2</f>
         <v>https://ror.org/00rqy9422</v>
+      </c>
+      <c r="H2" s="15" t="str">
+        <f>LICENSES!A2</f>
+        <v>https://creativecommons.org/licenses/by/4.0/</v>
       </c>
     </row>
   </sheetData>
@@ -1369,26 +1380,26 @@
     <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
-        <v>11</v>
+      <c r="C1" s="20" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1417,26 +1428,26 @@
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
-        <v>11</v>
+      <c r="C1" s="20" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>35</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1463,38 +1474,38 @@
     <col min="6" max="6" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="21" t="s">
+      <c r="C1" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>19</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>22</v>
-      </c>
       <c r="D2" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E2" s="16" t="b">
         <v>1</v>
@@ -1528,27 +1539,27 @@
     <col min="7" max="7" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:7" s="20" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="20" t="s">
+      <c r="C1" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>51</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1557,21 +1568,21 @@
         <v>#Speaker_01</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" s="17">
         <v>1979</v>
       </c>
-      <c r="G2" s="23"/>
+      <c r="G2" s="22"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C16" s="7"/>
@@ -2161,9 +2172,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2174,42 +2185,42 @@
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="12.83203125" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="40.1640625" customWidth="1"/>
     <col min="10" max="10" width="34.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="I1" s="21" t="s">
+      <c r="C1" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="21" t="s">
-        <v>23</v>
+      <c r="E1" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -2221,19 +2232,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E2" s="15" t="str">
         <f>SUBSTITUTE(_xlfn.CONCAT("#",F2)," ","_")</f>
         <v>#Speaker_01</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="18">
+        <v>40</v>
+      </c>
+      <c r="G2" s="23">
         <v>45455</v>
       </c>
       <c r="H2" s="15" t="str">
@@ -2241,10 +2252,10 @@
         <v>./</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -2554,7 +2565,7 @@
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2565,36 +2576,36 @@
     <col min="5" max="5" width="7.33203125" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="7" max="7" width="28.1640625" customWidth="1"/>
-    <col min="8" max="8" width="31" customWidth="1"/>
+    <col min="8" max="8" width="36.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="21" t="s">
+      <c r="G1" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="20" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2607,13 +2618,13 @@
         <v>3</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F2" s="16" t="b">
         <v>1</v>
@@ -2623,7 +2634,7 @@
         <v>#ExampleCollection_Speaker_01</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="I2" s="15" t="str">
         <f>G2</f>
@@ -2642,7 +2653,7 @@
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2654,36 +2665,36 @@
     <col min="5" max="5" width="7.33203125" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="7" max="7" width="28.1640625" customWidth="1"/>
-    <col min="8" max="8" width="31" customWidth="1"/>
+    <col min="8" max="8" width="36.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="21" t="s">
+      <c r="G1" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="20" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2696,13 +2707,13 @@
         <v>3</v>
       </c>
       <c r="C2" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>38</v>
-      </c>
       <c r="E2" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="16" t="b">
         <v>1</v>
@@ -2712,7 +2723,7 @@
         <v>#ExampleCollection_Speaker_01</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="I2" s="15" t="str">
         <f>G2</f>
@@ -2908,7 +2919,7 @@
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2922,29 +2933,29 @@
     <col min="7" max="8" width="28.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="21" t="s">
+      <c r="F1" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="20" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2957,13 +2968,13 @@
         <v>3</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" s="16" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
places section added, template updated
</commit_message>
<xml_diff>
--- a/content/resources/user-guides/crate-o/spreadsheet-upload/ro-crate-metadata-template.xlsx
+++ b/content/resources/user-guides/crate-o/spreadsheet-upload/ro-crate-metadata-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rosannasmith/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uq-my.sharepoint.com/personal/uqrsmi37_uq_edu_au/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01926BD-2AF4-F740-AC3D-FF32CD4078D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="4_{92CF65D0-6DDF-1A4E-83D8-84FDF4AF32E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8B82A40-DC4C-DA48-824C-C43D8C62EFEE}"/>
   <bookViews>
-    <workbookView xWindow="5940" yWindow="5280" windowWidth="32900" windowHeight="20220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17940" yWindow="8680" windowWidth="26160" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="10" r:id="rId1"/>
@@ -18,11 +18,16 @@
     <sheet name="PUBLISHERS" sheetId="11" r:id="rId3"/>
     <sheet name="LICENSES" sheetId="8" r:id="rId4"/>
     <sheet name="PEOPLE" sheetId="7" r:id="rId5"/>
-    <sheet name="OBJECTS" sheetId="1" r:id="rId6"/>
-    <sheet name="CSV_FILES" sheetId="9" r:id="rId7"/>
-    <sheet name="EAF_FILES" sheetId="2" r:id="rId8"/>
-    <sheet name="WAV_FILES" sheetId="3" r:id="rId9"/>
+    <sheet name="PLACES" sheetId="14" r:id="rId6"/>
+    <sheet name="LOCALITIES" sheetId="13" r:id="rId7"/>
+    <sheet name="OBJECTS" sheetId="1" r:id="rId8"/>
+    <sheet name="CSV_FILES" sheetId="9" r:id="rId9"/>
+    <sheet name="EAF_FILES" sheetId="2" r:id="rId10"/>
+    <sheet name="WAV_FILES" sheetId="3" r:id="rId11"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">OBJECTS!$A$1:$K$2</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -41,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="68">
   <si>
     <t>@id</t>
   </si>
@@ -187,9 +192,6 @@
     <t>CSV/ExampleCollection_Speaker_01.csv</t>
   </si>
   <si>
-    <t>isRef_pdcm:memberOf</t>
-  </si>
-  <si>
     <t>language_code</t>
   </si>
   <si>
@@ -209,16 +211,52 @@
   </si>
   <si>
     <t>isRef_isPartOf</t>
+  </si>
+  <si>
+    <t>2024-09-04</t>
+  </si>
+  <si>
+    <t>isRef_pcdm:memberOf</t>
+  </si>
+  <si>
+    <t>asWKT</t>
+  </si>
+  <si>
+    <t>#Location-1</t>
+  </si>
+  <si>
+    <t>Geometry</t>
+  </si>
+  <si>
+    <t>.latitude</t>
+  </si>
+  <si>
+    <t>.longitude</t>
+  </si>
+  <si>
+    <t>isRef_contentLocation</t>
+  </si>
+  <si>
+    <t>isRef_geo</t>
+  </si>
+  <si>
+    <t>Place</t>
+  </si>
+  <si>
+    <t>#Place-1</t>
+  </si>
+  <si>
+    <t>Naarm</t>
+  </si>
+  <si>
+    <t>Traditional Place name of Melbourne.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-  </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -424,6 +462,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="8" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="43">
     <fill>
@@ -860,7 +905,7 @@
     <xf numFmtId="0" fontId="23" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="57"/>
@@ -908,7 +953,9 @@
     <xf numFmtId="0" fontId="16" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="27" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="27" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="58">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1286,11 +1333,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B1B4B01-7DA1-4F69-8EF2-3B9D5666F67A}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1302,9 +1349,10 @@
     <col min="6" max="6" width="11.6640625" customWidth="1"/>
     <col min="7" max="7" width="22.6640625" customWidth="1"/>
     <col min="8" max="8" width="40.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1329,8 +1377,11 @@
       <c r="H1" s="20" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>27</v>
       </c>
@@ -1358,9 +1409,537 @@
         <f>LICENSES!A2</f>
         <v>https://creativecommons.org/licenses/by/4.0/</v>
       </c>
+      <c r="I2" s="23" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:J61"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40.5" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="28.1640625" customWidth="1"/>
+    <col min="8" max="8" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="str">
+        <f>_xlfn.CONCAT(C2,"/",_xlfn.CONCAT(D2,E2))</f>
+        <v>Transcripts/ExampleCollection_Speaker_01.eaf</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="15" t="str">
+        <f>_xlfn.CONCAT("#",D2)</f>
+        <v>#ExampleCollection_Speaker_01</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="15" t="str">
+        <f>G2</f>
+        <v>#ExampleCollection_Speaker_01</v>
+      </c>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J24" s="2"/>
+    </row>
+    <row r="25" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J28" s="2"/>
+    </row>
+    <row r="29" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J29" s="2"/>
+    </row>
+    <row r="30" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J30" s="2"/>
+    </row>
+    <row r="31" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J32" s="2"/>
+    </row>
+    <row r="33" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J33" s="2"/>
+    </row>
+    <row r="34" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J34" s="2"/>
+    </row>
+    <row r="35" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J35" s="2"/>
+    </row>
+    <row r="36" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J36" s="2"/>
+    </row>
+    <row r="37" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J37" s="2"/>
+    </row>
+    <row r="38" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J38" s="2"/>
+    </row>
+    <row r="39" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J39" s="2"/>
+    </row>
+    <row r="40" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J40" s="2"/>
+    </row>
+    <row r="41" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J41" s="2"/>
+    </row>
+    <row r="42" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J42" s="2"/>
+    </row>
+    <row r="43" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J43" s="2"/>
+    </row>
+    <row r="44" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J44" s="2"/>
+    </row>
+    <row r="45" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J45" s="2"/>
+    </row>
+    <row r="46" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J46" s="2"/>
+    </row>
+    <row r="47" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J47" s="2"/>
+    </row>
+    <row r="48" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J48" s="2"/>
+    </row>
+    <row r="49" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J49" s="2"/>
+    </row>
+    <row r="50" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J50" s="2"/>
+    </row>
+    <row r="51" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J51" s="2"/>
+    </row>
+    <row r="52" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J52" s="2"/>
+    </row>
+    <row r="53" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J53" s="2"/>
+    </row>
+    <row r="54" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J54" s="2"/>
+    </row>
+    <row r="55" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J55" s="2"/>
+    </row>
+    <row r="56" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J56" s="2"/>
+    </row>
+    <row r="57" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J57" s="2"/>
+    </row>
+    <row r="58" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J58" s="2"/>
+    </row>
+    <row r="59" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J59" s="2"/>
+    </row>
+    <row r="60" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J60" s="2"/>
+    </row>
+    <row r="61" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J61" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:I61"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="36.6640625" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" customWidth="1"/>
+    <col min="7" max="8" width="28.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="str">
+        <f>_xlfn.CONCAT(C2,"/",_xlfn.CONCAT(D2,E2))</f>
+        <v>Audio/ExampleCollection_Speaker_01.wav</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="15" t="str">
+        <f>_xlfn.CONCAT("#",D2)</f>
+        <v>#ExampleCollection_Speaker_01</v>
+      </c>
+      <c r="H2" s="15" t="str">
+        <f>G2</f>
+        <v>#ExampleCollection_Speaker_01</v>
+      </c>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I30" s="2"/>
+    </row>
+    <row r="31" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I31" s="2"/>
+    </row>
+    <row r="32" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I32" s="2"/>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I33" s="2"/>
+    </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I34" s="2"/>
+    </row>
+    <row r="35" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I35" s="2"/>
+    </row>
+    <row r="36" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I36" s="2"/>
+    </row>
+    <row r="37" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I37" s="2"/>
+    </row>
+    <row r="38" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I38" s="2"/>
+    </row>
+    <row r="39" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I39" s="2"/>
+    </row>
+    <row r="40" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I40" s="2"/>
+    </row>
+    <row r="41" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I41" s="2"/>
+    </row>
+    <row r="42" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I42" s="2"/>
+    </row>
+    <row r="43" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I43" s="2"/>
+    </row>
+    <row r="44" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I44" s="2"/>
+    </row>
+    <row r="45" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I45" s="2"/>
+    </row>
+    <row r="46" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I46" s="2"/>
+    </row>
+    <row r="47" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I47" s="2"/>
+    </row>
+    <row r="48" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I48" s="2"/>
+    </row>
+    <row r="49" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I49" s="2"/>
+    </row>
+    <row r="50" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I50" s="2"/>
+    </row>
+    <row r="51" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I51" s="2"/>
+    </row>
+    <row r="52" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I52" s="2"/>
+    </row>
+    <row r="53" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I53" s="2"/>
+    </row>
+    <row r="54" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I54" s="2"/>
+    </row>
+    <row r="55" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I55" s="2"/>
+    </row>
+    <row r="56" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I56" s="2"/>
+    </row>
+    <row r="57" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I57" s="2"/>
+    </row>
+    <row r="58" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I58" s="2"/>
+    </row>
+    <row r="59" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I59" s="2"/>
+    </row>
+    <row r="60" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I60" s="2"/>
+    </row>
+    <row r="61" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I61" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1499,13 +2078,13 @@
         <v>20</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E2" s="16" t="b">
         <v>1</v>
@@ -1525,7 +2104,7 @@
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1550,7 +2129,7 @@
         <v>10</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>46</v>
@@ -1559,7 +2138,7 @@
         <v>9</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1574,7 +2153,7 @@
         <v>40</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>6</v>
@@ -2169,10 +2748,125 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662AD084-ACEE-B548-980B-57F8B669CD21}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="20" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53972FEC-5747-7342-B007-022E1CF432E7}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="20" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="24">
+        <v>-37.799999999999997</v>
+      </c>
+      <c r="D2" s="24">
+        <v>144.9</v>
+      </c>
+      <c r="E2" s="25" t="str">
+        <f>_xlfn.CONCAT("POINT(",D2," ",C2,")")</f>
+        <v>POINT(144.9 -37.8)</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K61"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
@@ -2185,13 +2879,14 @@
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="12.83203125" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="40.1640625" customWidth="1"/>
     <col min="10" max="10" width="34.33203125" customWidth="1"/>
+    <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -2214,7 +2909,7 @@
         <v>12</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="I1" s="20" t="s">
         <v>16</v>
@@ -2222,8 +2917,11 @@
       <c r="J1" s="20" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" s="20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="str">
         <f>_xlfn.CONCAT("#",C2)</f>
         <v>#ExampleCollection_Speaker_01</v>
@@ -2244,8 +2942,8 @@
       <c r="F2" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="23">
-        <v>45455</v>
+      <c r="G2" s="23" t="s">
+        <v>55</v>
       </c>
       <c r="H2" s="15" t="str">
         <f>ROOT!A2</f>
@@ -2257,73 +2955,76 @@
       <c r="J2" s="16" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2" s="24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G3" s="1"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G4" s="1"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G5" s="1"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G6" s="1"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G7" s="1"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G8" s="1"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G9" s="1"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G10" s="1"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G11" s="1"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G12" s="1"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G13" s="1"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G14" s="1"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G15" s="1"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G16" s="1"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -2559,11 +3260,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2247A9B1-0E03-4A4A-BFED-598B9B7CC7C6}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
@@ -2600,7 +3301,7 @@
         <v>15</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H1" s="20" t="s">
         <v>5</v>
@@ -2634,537 +3335,12 @@
         <v>#ExampleCollection_Speaker_01</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I2" s="15" t="str">
         <f>G2</f>
         <v>#ExampleCollection_Speaker_01</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J61"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="40.5" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" customWidth="1"/>
-    <col min="4" max="4" width="27.1640625" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="28.1640625" customWidth="1"/>
-    <col min="8" max="8" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="20" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="str">
-        <f>_xlfn.CONCAT(C2,"/",_xlfn.CONCAT(D2,E2))</f>
-        <v>Transcripts/ExampleCollection_Speaker_01.eaf</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" s="15" t="str">
-        <f>_xlfn.CONCAT("#",D2)</f>
-        <v>#ExampleCollection_Speaker_01</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="15" t="str">
-        <f>G2</f>
-        <v>#ExampleCollection_Speaker_01</v>
-      </c>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J25" s="2"/>
-    </row>
-    <row r="26" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J27" s="2"/>
-    </row>
-    <row r="28" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J30" s="2"/>
-    </row>
-    <row r="31" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J31" s="2"/>
-    </row>
-    <row r="32" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J32" s="2"/>
-    </row>
-    <row r="33" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J33" s="2"/>
-    </row>
-    <row r="34" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J34" s="2"/>
-    </row>
-    <row r="35" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J35" s="2"/>
-    </row>
-    <row r="36" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J36" s="2"/>
-    </row>
-    <row r="37" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J37" s="2"/>
-    </row>
-    <row r="38" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J38" s="2"/>
-    </row>
-    <row r="39" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J39" s="2"/>
-    </row>
-    <row r="40" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J40" s="2"/>
-    </row>
-    <row r="41" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J41" s="2"/>
-    </row>
-    <row r="42" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J42" s="2"/>
-    </row>
-    <row r="43" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J43" s="2"/>
-    </row>
-    <row r="44" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J44" s="2"/>
-    </row>
-    <row r="45" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J45" s="2"/>
-    </row>
-    <row r="46" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J46" s="2"/>
-    </row>
-    <row r="47" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J47" s="2"/>
-    </row>
-    <row r="48" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J48" s="2"/>
-    </row>
-    <row r="49" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J49" s="2"/>
-    </row>
-    <row r="50" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J50" s="2"/>
-    </row>
-    <row r="51" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J51" s="2"/>
-    </row>
-    <row r="52" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J52" s="2"/>
-    </row>
-    <row r="53" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J53" s="2"/>
-    </row>
-    <row r="54" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J54" s="2"/>
-    </row>
-    <row r="55" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J55" s="2"/>
-    </row>
-    <row r="56" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J56" s="2"/>
-    </row>
-    <row r="57" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J57" s="2"/>
-    </row>
-    <row r="58" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J58" s="2"/>
-    </row>
-    <row r="59" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J59" s="2"/>
-    </row>
-    <row r="60" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J60" s="2"/>
-    </row>
-    <row r="61" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J61" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I61"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="36.6640625" customWidth="1"/>
-    <col min="2" max="2" width="6.5" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" customWidth="1"/>
-    <col min="4" max="4" width="27.1640625" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" customWidth="1"/>
-    <col min="6" max="6" width="21.1640625" customWidth="1"/>
-    <col min="7" max="8" width="28.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="str">
-        <f>_xlfn.CONCAT(C2,"/",_xlfn.CONCAT(D2,E2))</f>
-        <v>Audio/ExampleCollection_Speaker_01.wav</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" s="15" t="str">
-        <f>_xlfn.CONCAT("#",D2)</f>
-        <v>#ExampleCollection_Speaker_01</v>
-      </c>
-      <c r="H2" s="15" t="str">
-        <f>G2</f>
-        <v>#ExampleCollection_Speaker_01</v>
-      </c>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I23" s="2"/>
-    </row>
-    <row r="24" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I24" s="2"/>
-    </row>
-    <row r="25" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I25" s="2"/>
-    </row>
-    <row r="26" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I26" s="2"/>
-    </row>
-    <row r="27" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I27" s="2"/>
-    </row>
-    <row r="28" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I28" s="2"/>
-    </row>
-    <row r="29" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I29" s="2"/>
-    </row>
-    <row r="30" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I30" s="2"/>
-    </row>
-    <row r="31" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I31" s="2"/>
-    </row>
-    <row r="32" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I32" s="2"/>
-    </row>
-    <row r="33" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I33" s="2"/>
-    </row>
-    <row r="34" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I34" s="2"/>
-    </row>
-    <row r="35" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I35" s="2"/>
-    </row>
-    <row r="36" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I36" s="2"/>
-    </row>
-    <row r="37" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I37" s="2"/>
-    </row>
-    <row r="38" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I38" s="2"/>
-    </row>
-    <row r="39" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I39" s="2"/>
-    </row>
-    <row r="40" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I40" s="2"/>
-    </row>
-    <row r="41" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I41" s="2"/>
-    </row>
-    <row r="42" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I42" s="2"/>
-    </row>
-    <row r="43" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I43" s="2"/>
-    </row>
-    <row r="44" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I44" s="2"/>
-    </row>
-    <row r="45" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I45" s="2"/>
-    </row>
-    <row r="46" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I46" s="2"/>
-    </row>
-    <row r="47" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I47" s="2"/>
-    </row>
-    <row r="48" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I48" s="2"/>
-    </row>
-    <row r="49" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I49" s="2"/>
-    </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I50" s="2"/>
-    </row>
-    <row r="51" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I51" s="2"/>
-    </row>
-    <row r="52" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I52" s="2"/>
-    </row>
-    <row r="53" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I53" s="2"/>
-    </row>
-    <row r="54" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I54" s="2"/>
-    </row>
-    <row r="55" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I55" s="2"/>
-    </row>
-    <row r="56" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I56" s="2"/>
-    </row>
-    <row r="57" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I57" s="2"/>
-    </row>
-    <row r="58" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I58" s="2"/>
-    </row>
-    <row r="59" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I59" s="2"/>
-    </row>
-    <row r="60" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I60" s="2"/>
-    </row>
-    <row r="61" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I61" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updates to cite data page and spreadsheet upload
</commit_message>
<xml_diff>
--- a/content/resources/user-guides/crate-o/spreadsheet-upload/ro-crate-metadata-template.xlsx
+++ b/content/resources/user-guides/crate-o/spreadsheet-upload/ro-crate-metadata-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uq-my.sharepoint.com/personal/uqrsmi37_uq_edu_au/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rosanna/Documents/Repos/ldaca-website/content/resources/user-guides/crate-o/spreadsheet-upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="4_{92CF65D0-6DDF-1A4E-83D8-84FDF4AF32E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8B82A40-DC4C-DA48-824C-C43D8C62EFEE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87A7B69-D91B-234A-AFBE-1DD8CB4DCA2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17940" yWindow="8680" windowWidth="26160" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22600" yWindow="9380" windowWidth="26160" windowHeight="15760" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="10" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="71">
   <si>
     <t>@id</t>
   </si>
@@ -192,12 +192,6 @@
     <t>CSV/ExampleCollection_Speaker_01.csv</t>
   </si>
   <si>
-    <t>language_code</t>
-  </si>
-  <si>
-    <t>stan1293</t>
-  </si>
-  <si>
     <t>isRef_specializationOf</t>
   </si>
   <si>
@@ -250,6 +244,21 @@
   </si>
   <si>
     <t>Traditional Place name of Melbourne.</t>
+  </si>
+  <si>
+    <t>inLanguage</t>
+  </si>
+  <si>
+    <t>subjectLanguage</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>doi</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1000/182</t>
   </si>
 </sst>
 </file>
@@ -905,7 +914,7 @@
     <xf numFmtId="0" fontId="23" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="57"/>
@@ -920,9 +929,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="54" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="51" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -933,12 +939,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="48" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="55" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="47" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1333,11 +1333,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B1B4B01-7DA1-4F69-8EF2-3B9D5666F67A}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1345,72 +1345,92 @@
     <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" customWidth="1"/>
-    <col min="5" max="5" width="25.5" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" customWidth="1"/>
-    <col min="8" max="8" width="40.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="25.5" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" customWidth="1"/>
+    <col min="9" max="9" width="40.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="H1" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="I1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="J1" s="17" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="K1" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="15" t="str">
+      <c r="F2" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="12" t="str">
         <f>AUTHORS!A2</f>
         <v>#LDaCA</v>
       </c>
-      <c r="G2" s="15" t="str">
+      <c r="H2" s="12" t="str">
         <f>PUBLISHERS!A2</f>
         <v>https://ror.org/00rqy9422</v>
       </c>
-      <c r="H2" s="15" t="str">
+      <c r="I2" s="12" t="str">
         <f>LICENSES!A2</f>
         <v>https://creativecommons.org/licenses/by/4.0/</v>
       </c>
-      <c r="I2" s="23" t="s">
-        <v>55</v>
+      <c r="J2" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1440,63 +1460,63 @@
     <col min="9" max="9" width="28.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="H1" s="20" t="s">
+      <c r="G1" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="str">
+      <c r="A2" s="12" t="str">
         <f>_xlfn.CONCAT(C2,"/",_xlfn.CONCAT(D2,E2))</f>
         <v>Transcripts/ExampleCollection_Speaker_01.eaf</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="16" t="b">
+      <c r="F2" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="G2" s="15" t="str">
+      <c r="G2" s="12" t="str">
         <f>_xlfn.CONCAT("#",D2)</f>
         <v>#ExampleCollection_Speaker_01</v>
       </c>
-      <c r="H2" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" s="15" t="str">
+      <c r="H2" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="12" t="str">
         <f>G2</f>
         <v>#ExampleCollection_Speaker_01</v>
       </c>
@@ -1704,57 +1724,57 @@
     <col min="7" max="8" width="28.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="H1" s="20" t="s">
+      <c r="G1" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="str">
+      <c r="A2" s="12" t="str">
         <f>_xlfn.CONCAT(C2,"/",_xlfn.CONCAT(D2,E2))</f>
         <v>Audio/ExampleCollection_Speaker_01.wav</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="16" t="b">
+      <c r="F2" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="G2" s="15" t="str">
+      <c r="G2" s="12" t="str">
         <f>_xlfn.CONCAT("#",D2)</f>
         <v>#ExampleCollection_Speaker_01</v>
       </c>
-      <c r="H2" s="15" t="str">
+      <c r="H2" s="12" t="str">
         <f>G2</f>
         <v>#ExampleCollection_Speaker_01</v>
       </c>
@@ -1959,25 +1979,25 @@
     <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="13" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2007,25 +2027,25 @@
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="13" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2053,43 +2073,43 @@
     <col min="6" max="6" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="16" t="s">
+      <c r="B2" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="16" t="b">
+      <c r="D2" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="F2" s="16" t="b">
+      <c r="F2" s="13" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2100,11 +2120,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABBB93A8-8994-2841-935E-D84C02300906}">
-  <dimension ref="A1:G175"/>
+  <dimension ref="A1:F175"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2112,635 +2132,482 @@
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
     <col min="2" max="2" width="6.6640625" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="9" style="5" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="9" style="5" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="20" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:6" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="str">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="str">
         <f t="shared" ref="A2" si="0">SUBSTITUTE(_xlfn.CONCAT("#",C2)," ","_")</f>
         <v>#Speaker_01</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="17" t="s">
+      <c r="D2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="17">
+      <c r="E2" s="14">
         <v>1979</v>
       </c>
-      <c r="G2" s="22"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F2" s="19"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-    </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-    </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-    </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-    </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-    </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-    </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D42" s="7"/>
-    </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D46" s="7"/>
-    </row>
-    <row r="47" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D47" s="7"/>
-    </row>
-    <row r="58" spans="4:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D58" s="8"/>
       <c r="E58" s="9"/>
-      <c r="F58" s="10"/>
-    </row>
-    <row r="59" spans="4:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D59" s="8"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="11"/>
-    </row>
-    <row r="60" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D60" s="8"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="11"/>
-    </row>
-    <row r="61" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E59" s="10"/>
+    </row>
+    <row r="60" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D60" s="11"/>
+      <c r="E60" s="10"/>
+    </row>
+    <row r="61" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D61" s="8"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="6"/>
-    </row>
-    <row r="62" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E61" s="6"/>
+    </row>
+    <row r="62" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D62" s="8"/>
       <c r="E62" s="9"/>
-      <c r="F62" s="10"/>
-    </row>
-    <row r="63" spans="4:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D63" s="8"/>
-      <c r="E63" s="9"/>
-      <c r="F63" s="11"/>
-    </row>
-    <row r="64" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D64" s="8"/>
-      <c r="E64" s="12"/>
-      <c r="F64" s="6"/>
-    </row>
-    <row r="65" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D65" s="13"/>
-      <c r="E65" s="9"/>
-      <c r="F65" s="11"/>
-    </row>
-    <row r="66" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E63" s="10"/>
+    </row>
+    <row r="64" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D64" s="11"/>
+      <c r="E64" s="6"/>
+    </row>
+    <row r="65" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D65" s="8"/>
+      <c r="E65" s="10"/>
+    </row>
+    <row r="66" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D66" s="8"/>
-      <c r="E66" s="9"/>
-      <c r="F66" s="11"/>
-    </row>
-    <row r="67" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E66" s="10"/>
+    </row>
+    <row r="67" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D67" s="8"/>
       <c r="E67" s="9"/>
-      <c r="F67" s="10"/>
-    </row>
-    <row r="68" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D68" s="8"/>
-      <c r="E68" s="12"/>
-      <c r="F68" s="6"/>
-    </row>
-    <row r="69" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D69" s="13"/>
-      <c r="E69" s="12"/>
-      <c r="F69" s="11"/>
-    </row>
-    <row r="70" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D70" s="14"/>
-      <c r="E70" s="12"/>
-      <c r="F70" s="11"/>
-    </row>
-    <row r="71" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D71" s="13"/>
-      <c r="E71" s="12"/>
-      <c r="F71" s="11"/>
-    </row>
-    <row r="72" spans="4:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D68" s="11"/>
+      <c r="E68" s="6"/>
+    </row>
+    <row r="69" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D69" s="11"/>
+      <c r="E69" s="10"/>
+    </row>
+    <row r="70" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D70" s="11"/>
+      <c r="E70" s="10"/>
+    </row>
+    <row r="71" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D71" s="11"/>
+      <c r="E71" s="10"/>
+    </row>
+    <row r="72" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D72" s="8"/>
-      <c r="E72" s="9"/>
-      <c r="F72" s="11"/>
-    </row>
-    <row r="73" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D73" s="13"/>
-      <c r="E73" s="9"/>
-      <c r="F73" s="11"/>
-    </row>
-    <row r="74" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D74" s="13"/>
-      <c r="E74" s="9"/>
-      <c r="F74" s="11"/>
-    </row>
-    <row r="75" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E72" s="10"/>
+    </row>
+    <row r="73" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D73" s="8"/>
+      <c r="E73" s="10"/>
+    </row>
+    <row r="74" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D74" s="8"/>
+      <c r="E74" s="10"/>
+    </row>
+    <row r="75" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D75" s="8"/>
-      <c r="E75" s="9"/>
-      <c r="F75" s="11"/>
-    </row>
-    <row r="76" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D76" s="13"/>
-      <c r="E76" s="12"/>
-      <c r="F76" s="11"/>
-    </row>
-    <row r="77" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D77" s="13"/>
+      <c r="E75" s="10"/>
+    </row>
+    <row r="76" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D76" s="11"/>
+      <c r="E76" s="10"/>
+    </row>
+    <row r="77" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D77" s="8"/>
       <c r="E77" s="9"/>
-      <c r="F77" s="10"/>
-    </row>
-    <row r="78" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D78" s="13"/>
-      <c r="E78" s="9"/>
-      <c r="F78" s="11"/>
-    </row>
-    <row r="79" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D79" s="14"/>
-      <c r="E79" s="12"/>
-      <c r="F79" s="11"/>
-    </row>
-    <row r="80" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D80" s="13"/>
-      <c r="E80" s="9"/>
-      <c r="F80" s="11"/>
-    </row>
-    <row r="81" spans="4:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D78" s="8"/>
+      <c r="E78" s="10"/>
+    </row>
+    <row r="79" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D79" s="11"/>
+      <c r="E79" s="10"/>
+    </row>
+    <row r="80" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D80" s="8"/>
+      <c r="E80" s="10"/>
+    </row>
+    <row r="81" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D81" s="8"/>
       <c r="E81" s="9"/>
-      <c r="F81" s="10"/>
-    </row>
-    <row r="82" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D82" s="8"/>
-      <c r="E82" s="12"/>
-      <c r="F82" s="6"/>
-    </row>
-    <row r="83" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D83" s="8"/>
-      <c r="E83" s="12"/>
-      <c r="F83" s="6"/>
-    </row>
-    <row r="84" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D84" s="13"/>
-      <c r="E84" s="9"/>
-      <c r="F84" s="11"/>
-    </row>
-    <row r="85" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D85" s="14"/>
-      <c r="E85" s="12"/>
-      <c r="F85" s="6"/>
-    </row>
-    <row r="86" spans="4:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D82" s="11"/>
+      <c r="E82" s="6"/>
+    </row>
+    <row r="83" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D83" s="11"/>
+      <c r="E83" s="6"/>
+    </row>
+    <row r="84" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D84" s="8"/>
+      <c r="E84" s="10"/>
+    </row>
+    <row r="85" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D85" s="11"/>
+      <c r="E85" s="6"/>
+    </row>
+    <row r="86" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D86" s="8"/>
-      <c r="E86" s="9"/>
-      <c r="F86" s="6"/>
-    </row>
-    <row r="87" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E86" s="6"/>
+    </row>
+    <row r="87" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D87" s="8"/>
-      <c r="E87" s="9"/>
-      <c r="F87" s="6"/>
-    </row>
-    <row r="88" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D88" s="13"/>
-      <c r="E88" s="9"/>
-      <c r="F88" s="11"/>
-    </row>
-    <row r="89" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D89" s="13"/>
-      <c r="E89" s="9"/>
-      <c r="F89" s="11"/>
-    </row>
-    <row r="90" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D90" s="13"/>
-      <c r="E90" s="9"/>
-      <c r="F90" s="11"/>
-    </row>
-    <row r="91" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D91" s="8"/>
-      <c r="E91" s="12"/>
-      <c r="F91" s="10"/>
-    </row>
-    <row r="92" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D92" s="14"/>
-      <c r="E92" s="9"/>
-      <c r="F92" s="11"/>
-    </row>
-    <row r="93" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D93" s="8"/>
-      <c r="E93" s="12"/>
-      <c r="F93" s="10"/>
-    </row>
-    <row r="94" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D94" s="13"/>
-      <c r="E94" s="12"/>
-      <c r="F94" s="11"/>
-    </row>
-    <row r="95" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D95" s="13"/>
-      <c r="E95" s="9"/>
-      <c r="F95" s="6"/>
-    </row>
-    <row r="96" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D96" s="8"/>
-      <c r="E96" s="12"/>
-      <c r="F96" s="6"/>
-    </row>
-    <row r="97" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D97" s="14"/>
-      <c r="E97" s="9"/>
-      <c r="F97" s="6"/>
-    </row>
-    <row r="98" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D98" s="13"/>
-      <c r="E98" s="12"/>
-      <c r="F98" s="11"/>
-    </row>
-    <row r="99" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D99" s="13"/>
-      <c r="E99" s="9"/>
-      <c r="F99" s="11"/>
-    </row>
-    <row r="100" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D100" s="13"/>
-      <c r="E100" s="12"/>
-      <c r="F100" s="11"/>
-    </row>
-    <row r="101" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D101" s="13"/>
-      <c r="E101" s="9"/>
-      <c r="F101" s="11"/>
-    </row>
-    <row r="102" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D102" s="8"/>
-      <c r="E102" s="12"/>
-      <c r="F102" s="10"/>
-    </row>
-    <row r="103" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D103" s="13"/>
-      <c r="E103" s="12"/>
-      <c r="F103" s="11"/>
-    </row>
-    <row r="104" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D104" s="14"/>
-      <c r="E104" s="12"/>
-      <c r="F104" s="6"/>
-    </row>
-    <row r="105" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D105" s="14"/>
-      <c r="E105" s="12"/>
-      <c r="F105" s="11"/>
-    </row>
-    <row r="106" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D106" s="8"/>
-      <c r="E106" s="12"/>
-      <c r="F106" s="6"/>
-    </row>
-    <row r="107" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D107" s="8"/>
-      <c r="E107" s="12"/>
-      <c r="F107" s="11"/>
-    </row>
-    <row r="108" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D108" s="13"/>
-      <c r="E108" s="12"/>
-      <c r="F108" s="11"/>
-    </row>
-    <row r="109" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D109" s="8"/>
-      <c r="E109" s="12"/>
-      <c r="F109" s="10"/>
-    </row>
-    <row r="110" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D110" s="13"/>
-      <c r="E110" s="12"/>
-      <c r="F110" s="11"/>
-    </row>
-    <row r="111" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D111" s="8"/>
-      <c r="E111" s="12"/>
-      <c r="F111" s="6"/>
-    </row>
-    <row r="112" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D112" s="14"/>
-      <c r="E112" s="9"/>
-      <c r="F112" s="11"/>
-    </row>
-    <row r="113" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D113" s="14"/>
-      <c r="E113" s="9"/>
-      <c r="F113" s="6"/>
-    </row>
-    <row r="114" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D114" s="13"/>
-      <c r="E114" s="12"/>
-      <c r="F114" s="11"/>
-    </row>
-    <row r="115" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D115" s="7"/>
-    </row>
-    <row r="116" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D116" s="7"/>
-    </row>
-    <row r="119" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="E87" s="6"/>
+    </row>
+    <row r="88" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D88" s="8"/>
+      <c r="E88" s="10"/>
+    </row>
+    <row r="89" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D89" s="8"/>
+      <c r="E89" s="10"/>
+    </row>
+    <row r="90" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D90" s="8"/>
+      <c r="E90" s="10"/>
+    </row>
+    <row r="91" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D91" s="11"/>
+      <c r="E91" s="9"/>
+    </row>
+    <row r="92" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D92" s="8"/>
+      <c r="E92" s="10"/>
+    </row>
+    <row r="93" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D93" s="11"/>
+      <c r="E93" s="9"/>
+    </row>
+    <row r="94" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D94" s="11"/>
+      <c r="E94" s="10"/>
+    </row>
+    <row r="95" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D95" s="8"/>
+      <c r="E95" s="6"/>
+    </row>
+    <row r="96" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D96" s="11"/>
+      <c r="E96" s="6"/>
+    </row>
+    <row r="97" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D97" s="8"/>
+      <c r="E97" s="6"/>
+    </row>
+    <row r="98" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D98" s="11"/>
+      <c r="E98" s="10"/>
+    </row>
+    <row r="99" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D99" s="8"/>
+      <c r="E99" s="10"/>
+    </row>
+    <row r="100" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D100" s="11"/>
+      <c r="E100" s="10"/>
+    </row>
+    <row r="101" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D101" s="8"/>
+      <c r="E101" s="10"/>
+    </row>
+    <row r="102" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D102" s="11"/>
+      <c r="E102" s="9"/>
+    </row>
+    <row r="103" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D103" s="11"/>
+      <c r="E103" s="10"/>
+    </row>
+    <row r="104" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D104" s="11"/>
+      <c r="E104" s="6"/>
+    </row>
+    <row r="105" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D105" s="11"/>
+      <c r="E105" s="10"/>
+    </row>
+    <row r="106" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D106" s="11"/>
+      <c r="E106" s="6"/>
+    </row>
+    <row r="107" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D107" s="11"/>
+      <c r="E107" s="10"/>
+    </row>
+    <row r="108" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D108" s="11"/>
+      <c r="E108" s="10"/>
+    </row>
+    <row r="109" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D109" s="11"/>
+      <c r="E109" s="9"/>
+    </row>
+    <row r="110" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D110" s="11"/>
+      <c r="E110" s="10"/>
+    </row>
+    <row r="111" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D111" s="11"/>
+      <c r="E111" s="6"/>
+    </row>
+    <row r="112" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D112" s="8"/>
+      <c r="E112" s="10"/>
+    </row>
+    <row r="113" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D113" s="8"/>
+      <c r="E113" s="6"/>
+    </row>
+    <row r="114" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D114" s="11"/>
+      <c r="E114" s="10"/>
+    </row>
+    <row r="119" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C119" s="7"/>
       <c r="D119" s="7"/>
       <c r="E119" s="7"/>
-      <c r="F119" s="7"/>
-    </row>
-    <row r="120" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="120" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C120" s="7"/>
       <c r="D120" s="7"/>
       <c r="E120" s="7"/>
-      <c r="F120" s="7"/>
-    </row>
-    <row r="121" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="121" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C121" s="7"/>
       <c r="D121" s="7"/>
       <c r="E121" s="7"/>
-      <c r="F121" s="7"/>
-    </row>
-    <row r="122" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="122" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C122" s="7"/>
       <c r="D122" s="7"/>
       <c r="E122" s="7"/>
-      <c r="F122" s="7"/>
-    </row>
-    <row r="123" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="123" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C123" s="7"/>
       <c r="D123" s="7"/>
       <c r="E123" s="7"/>
-      <c r="F123" s="7"/>
-    </row>
-    <row r="124" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="124" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C124" s="7"/>
       <c r="D124" s="7"/>
       <c r="E124" s="7"/>
-      <c r="F124" s="7"/>
-    </row>
-    <row r="126" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="126" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C126" s="7"/>
       <c r="D126" s="7"/>
       <c r="E126" s="7"/>
-      <c r="F126" s="7"/>
-    </row>
-    <row r="127" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D127" s="7"/>
-    </row>
-    <row r="129" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="129" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C129" s="7"/>
       <c r="D129" s="7"/>
       <c r="E129" s="7"/>
-      <c r="F129" s="7"/>
-    </row>
-    <row r="132" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="132" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C132" s="7"/>
       <c r="D132" s="7"/>
       <c r="E132" s="7"/>
-      <c r="F132" s="7"/>
-    </row>
-    <row r="134" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="134" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C134" s="7"/>
       <c r="D134" s="7"/>
       <c r="E134" s="7"/>
-      <c r="F134" s="7"/>
-    </row>
-    <row r="137" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D137" s="7"/>
-    </row>
-    <row r="138" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D138" s="7"/>
-    </row>
-    <row r="141" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="141" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C141" s="7"/>
       <c r="D141" s="7"/>
       <c r="E141" s="7"/>
-      <c r="F141" s="7"/>
-    </row>
-    <row r="142" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="142" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C142" s="7"/>
       <c r="D142" s="7"/>
       <c r="E142" s="7"/>
-      <c r="F142" s="7"/>
-    </row>
-    <row r="143" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="143" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C143" s="7"/>
       <c r="D143" s="7"/>
       <c r="E143" s="7"/>
-      <c r="F143" s="7"/>
-    </row>
-    <row r="144" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="144" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C144" s="7"/>
       <c r="D144" s="7"/>
       <c r="E144" s="7"/>
-      <c r="F144" s="7"/>
-    </row>
-    <row r="145" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="145" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C145" s="7"/>
       <c r="D145" s="7"/>
       <c r="E145" s="7"/>
-      <c r="F145" s="7"/>
-    </row>
-    <row r="146" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D146" s="7"/>
-    </row>
-    <row r="147" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="147" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C147" s="7"/>
       <c r="D147" s="7"/>
       <c r="E147" s="7"/>
-      <c r="F147" s="7"/>
-    </row>
-    <row r="150" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D150" s="7"/>
-    </row>
-    <row r="151" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="151" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C151" s="7"/>
       <c r="D151" s="7"/>
       <c r="E151" s="7"/>
-      <c r="F151" s="7"/>
-    </row>
-    <row r="152" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="152" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C152" s="7"/>
       <c r="D152" s="7"/>
       <c r="E152" s="7"/>
-      <c r="F152" s="7"/>
-    </row>
-    <row r="153" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="153" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C153" s="7"/>
       <c r="D153" s="7"/>
       <c r="E153" s="7"/>
-      <c r="F153" s="7"/>
-    </row>
-    <row r="154" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="154" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C154" s="7"/>
       <c r="D154" s="7"/>
       <c r="E154" s="7"/>
-      <c r="F154" s="7"/>
-    </row>
-    <row r="155" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="155" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C155" s="7"/>
       <c r="D155" s="7"/>
       <c r="E155" s="7"/>
-      <c r="F155" s="7"/>
-    </row>
-    <row r="156" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D156" s="7"/>
-    </row>
-    <row r="158" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D158" s="7"/>
-    </row>
-    <row r="159" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="159" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C159" s="7"/>
       <c r="D159" s="7"/>
       <c r="E159" s="7"/>
-      <c r="F159" s="7"/>
-    </row>
-    <row r="160" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="160" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C160" s="7"/>
       <c r="D160" s="7"/>
       <c r="E160" s="7"/>
-      <c r="F160" s="7"/>
-    </row>
-    <row r="161" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="161" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C161" s="7"/>
       <c r="D161" s="7"/>
       <c r="E161" s="7"/>
-      <c r="F161" s="7"/>
-    </row>
-    <row r="162" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D162" s="7"/>
-    </row>
-    <row r="163" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D163" s="7"/>
-    </row>
-    <row r="165" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="165" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C165" s="7"/>
       <c r="D165" s="7"/>
       <c r="E165" s="7"/>
-      <c r="F165" s="7"/>
-    </row>
-    <row r="166" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="166" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C166" s="7"/>
       <c r="D166" s="7"/>
       <c r="E166" s="7"/>
-      <c r="F166" s="7"/>
-    </row>
-    <row r="167" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D167" s="7"/>
-    </row>
-    <row r="169" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="169" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C169" s="7"/>
       <c r="D169" s="7"/>
       <c r="E169" s="7"/>
-      <c r="F169" s="7"/>
-    </row>
-    <row r="170" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D170" s="7"/>
-    </row>
-    <row r="172" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="172" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C172" s="7"/>
       <c r="D172" s="7"/>
       <c r="E172" s="7"/>
-      <c r="F172" s="7"/>
-    </row>
-    <row r="173" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="173" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C173" s="7"/>
       <c r="D173" s="7"/>
       <c r="E173" s="7"/>
-      <c r="F173" s="7"/>
-    </row>
-    <row r="174" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="174" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C174" s="7"/>
       <c r="D174" s="7"/>
       <c r="E174" s="7"/>
-      <c r="F174" s="7"/>
-    </row>
-    <row r="175" spans="3:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="175" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C175" s="7"/>
       <c r="D175" s="7"/>
       <c r="E175" s="7"/>
-      <c r="F175" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2751,52 +2618,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662AD084-ACEE-B548-980B-57F8B669CD21}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="20" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:7" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
+      <c r="E1" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>58</v>
+      <c r="E2" s="21" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2809,7 +2676,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2819,40 +2686,40 @@
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="20" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:8" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="19" t="s">
+      <c r="C1" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="24">
+      <c r="C2" s="21">
         <v>-37.799999999999997</v>
       </c>
-      <c r="D2" s="24">
+      <c r="D2" s="21">
         <v>144.9</v>
       </c>
-      <c r="E2" s="25" t="str">
+      <c r="E2" s="22" t="str">
         <f>_xlfn.CONCAT("POINT(",D2," ",C2,")")</f>
         <v>POINT(144.9 -37.8)</v>
       </c>
@@ -2864,11 +2731,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K61"/>
+  <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2884,147 +2751,161 @@
     <col min="9" max="9" width="40.1640625" customWidth="1"/>
     <col min="10" max="10" width="34.33203125" customWidth="1"/>
     <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" s="20" t="s">
+      <c r="H1" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="20" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="str">
+      <c r="K1" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="str">
         <f>_xlfn.CONCAT("#",C2)</f>
         <v>#ExampleCollection_Speaker_01</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="15" t="str">
+      <c r="E2" s="12" t="str">
         <f>SUBSTITUTE(_xlfn.CONCAT("#",F2)," ","_")</f>
         <v>#Speaker_01</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" s="15" t="str">
+      <c r="G2" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="12" t="str">
         <f>ROOT!A2</f>
         <v>./</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K2" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" t="s">
+        <v>68</v>
+      </c>
+      <c r="M2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G3" s="1"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G4" s="1"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G5" s="1"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G6" s="1"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G7" s="1"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G8" s="1"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G9" s="1"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G10" s="1"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G11" s="1"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G12" s="1"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G13" s="1"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G14" s="1"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G15" s="1"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G16" s="1"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -3281,63 +3162,63 @@
     <col min="9" max="9" width="28.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="H1" s="20" t="s">
+      <c r="G1" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="str">
+      <c r="A2" s="12" t="str">
         <f>_xlfn.CONCAT(C2,"/",_xlfn.CONCAT(D2,E2))</f>
         <v>CSV/ExampleCollection_Speaker_01.csv</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="16" t="b">
+      <c r="F2" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="G2" s="15" t="str">
+      <c r="G2" s="12" t="str">
         <f>_xlfn.CONCAT("#",D2)</f>
         <v>#ExampleCollection_Speaker_01</v>
       </c>
-      <c r="H2" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" s="15" t="str">
+      <c r="H2" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="12" t="str">
         <f>G2</f>
         <v>#ExampleCollection_Speaker_01</v>
       </c>

</xml_diff>